<commit_message>
Add basic handling of photos provided in image archive
</commit_message>
<xml_diff>
--- a/utils/testdata/DigitalSafariTESTDATA.xlsx
+++ b/utils/testdata/DigitalSafariTESTDATA.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Data overview" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="423">
   <si>
     <t xml:space="preserve">Information for Digital Safari web app</t>
   </si>
@@ -832,6 +832,12 @@
   </si>
   <si>
     <t xml:space="preserve">Image ref</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bob</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jones</t>
   </si>
   <si>
     <t xml:space="preserve">Millport</t>
@@ -1980,7 +1986,7 @@
   </sheetPr>
   <dimension ref="A2:I46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I23" activeCellId="0" sqref="I23"/>
     </sheetView>
   </sheetViews>
@@ -3707,8 +3713,8 @@
   </sheetPr>
   <dimension ref="A3:K25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3777,32 +3783,36 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="118.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9"/>
+      <c r="A5" s="9" t="s">
+        <v>263</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>264</v>
+      </c>
       <c r="C5" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="E5" s="54" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="F5" s="54" t="n">
         <v>-4.92252593043097</v>
       </c>
       <c r="G5" s="33" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="H5" s="40" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="I5" s="55" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="J5" s="9"/>
       <c r="K5" s="9" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3812,26 +3822,26 @@
         <v>42</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="E6" s="56" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="F6" s="56" t="n">
         <v>-4.86914977337635</v>
       </c>
       <c r="G6" s="18" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="H6" s="35" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="J6" s="9"/>
       <c r="K6" s="9" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="53.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3841,7 +3851,7 @@
         <v>42</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="E7" s="56" t="n">
         <v>55.6129152128045</v>
@@ -3850,17 +3860,17 @@
         <v>-4.48937852433251</v>
       </c>
       <c r="G7" s="18" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="H7" s="35" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="I7" s="57" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="J7" s="9"/>
       <c r="K7" s="9" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3870,26 +3880,26 @@
         <v>42</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="E8" s="56" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="F8" s="56" t="n">
         <v>-4.68434127824148</v>
       </c>
       <c r="G8" s="18" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="H8" s="35" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="J8" s="9"/>
       <c r="K8" s="9" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="43.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3899,26 +3909,26 @@
         <v>42</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="E9" s="56" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="F9" s="56" t="n">
         <v>-4.66607004947121</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="H9" s="35" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="I9" s="57" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="J9" s="9"/>
       <c r="K9" s="9" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="53.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3928,26 +3938,26 @@
         <v>42</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="E10" s="56" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="F10" s="56" t="n">
         <v>-4.84348802802478</v>
       </c>
       <c r="G10" s="18" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="H10" s="35" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="I10" s="57" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="J10" s="9"/>
       <c r="K10" s="9" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3957,26 +3967,26 @@
         <v>42</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="E11" s="56" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="F11" s="56" t="n">
         <v>-4.28600140104111</v>
       </c>
       <c r="G11" s="18" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="H11" s="35" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="J11" s="9"/>
       <c r="K11" s="9" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="43.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3986,22 +3996,22 @@
         <v>42</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="E12" s="56" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="F12" s="56" t="n">
         <v>-4.69848050344589</v>
       </c>
       <c r="G12" s="18" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="H12" s="35" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="I12" s="57" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="J12" s="9"/>
       <c r="K12" s="9" t="s">
@@ -4015,22 +4025,22 @@
         <v>42</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="E13" s="56" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="F13" s="56" t="n">
         <v>-4.74514981453443</v>
       </c>
       <c r="G13" s="18" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="H13" s="35" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="I13" s="57" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="J13" s="9"/>
       <c r="K13" s="9" t="s">
@@ -4044,22 +4054,22 @@
         <v>42</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="E14" s="56" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="F14" s="56" t="n">
         <v>-4.73272769919101</v>
       </c>
       <c r="G14" s="18" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="H14" s="35" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="J14" s="9"/>
       <c r="K14" s="9" t="s">
@@ -4073,26 +4083,26 @@
         <v>42</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="E15" s="56" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="F15" s="56" t="n">
         <v>-5.19201756110202</v>
       </c>
       <c r="G15" s="18" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="H15" s="35" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="I15" s="57" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="J15" s="9"/>
       <c r="K15" s="9" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="85.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4102,26 +4112,26 @@
         <v>42</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="E16" s="56" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="F16" s="56" t="n">
         <v>-4.45465267405307</v>
       </c>
       <c r="G16" s="18" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="H16" s="35" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="I16" s="57" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="J16" s="9"/>
       <c r="K16" s="9" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4131,26 +4141,26 @@
         <v>42</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="E17" s="56" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="F17" s="56" t="n">
         <v>-4.47766172987618</v>
       </c>
       <c r="G17" s="18" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="H17" s="35" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="I17" s="57" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="J17" s="9"/>
       <c r="K17" s="9" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4346,7 +4356,7 @@
         <v>58</v>
       </c>
       <c r="I4" s="62" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="J4" s="63" t="s">
         <v>262</v>
@@ -4359,112 +4369,112 @@
       <c r="A5" s="65"/>
       <c r="B5" s="65"/>
       <c r="C5" s="65" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="D5" s="65" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="E5" s="65" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="F5" s="65" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="G5" s="66" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="H5" s="67" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="I5" s="68" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="J5" s="9"/>
       <c r="K5" s="9" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="53.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="69"/>
       <c r="B6" s="69"/>
       <c r="C6" s="69" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="D6" s="69" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="E6" s="69" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="F6" s="69" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="G6" s="69" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="H6" s="70" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="I6" s="36" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="J6" s="9"/>
       <c r="K6" s="9" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="64.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="69"/>
       <c r="B7" s="69"/>
       <c r="C7" s="69" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="D7" s="69" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="E7" s="69" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="F7" s="69" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="G7" s="69" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="H7" s="70" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="I7" s="36" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="J7" s="9"/>
       <c r="K7" s="9" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="69"/>
       <c r="B8" s="69"/>
       <c r="C8" s="69" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="D8" s="69" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="E8" s="69" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="F8" s="69" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="G8" s="71" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="H8" s="70" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="I8" s="36" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="J8" s="9"/>
       <c r="K8" s="9" t="s">
@@ -4475,87 +4485,87 @@
       <c r="A9" s="69"/>
       <c r="B9" s="69"/>
       <c r="C9" s="69" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="D9" s="69" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="E9" s="69" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="F9" s="69" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="G9" s="71" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="H9" s="70" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="I9" s="36" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="J9" s="9"/>
       <c r="K9" s="9" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="85.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="69"/>
       <c r="B10" s="69"/>
       <c r="C10" s="69" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="D10" s="69" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="E10" s="69" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="F10" s="69" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="G10" s="71" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="H10" s="70" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="I10" s="36" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="J10" s="9"/>
       <c r="K10" s="9" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="53.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="69"/>
       <c r="B11" s="69"/>
       <c r="C11" s="69" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="D11" s="69" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="E11" s="69" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="F11" s="69" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="G11" s="71" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="H11" s="70" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="I11" s="72" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="J11" s="9"/>
       <c r="K11" s="9" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4565,51 +4575,51 @@
         <v>43</v>
       </c>
       <c r="D12" s="69" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="E12" s="69" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="F12" s="69" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="G12" s="71" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="H12" s="70" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="I12" s="36" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="J12" s="9"/>
       <c r="K12" s="9" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="85.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="69"/>
       <c r="B13" s="69"/>
       <c r="C13" s="69" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="D13" s="69" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="E13" s="69" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="F13" s="69" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="G13" s="71" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="H13" s="70" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="I13" s="36" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="J13" s="9"/>
       <c r="K13" s="9" t="s">
@@ -4623,142 +4633,142 @@
         <v>43</v>
       </c>
       <c r="D14" s="69" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="E14" s="69" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="F14" s="69" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="G14" s="71" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="H14" s="70" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="I14" s="36" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="J14" s="9"/>
       <c r="K14" s="9" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="64.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="69"/>
       <c r="B15" s="69"/>
       <c r="C15" s="69" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="D15" s="69" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="E15" s="69" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="F15" s="69" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="G15" s="71" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="H15" s="70" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="I15" s="36" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="J15" s="9"/>
       <c r="K15" s="9" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="69"/>
       <c r="B16" s="69"/>
       <c r="C16" s="69" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="D16" s="69" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="E16" s="69" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="F16" s="69" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="G16" s="71" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="H16" s="70" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="I16" s="36" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="J16" s="9"/>
       <c r="K16" s="9" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="69"/>
       <c r="B17" s="69"/>
       <c r="C17" s="69" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="D17" s="69" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="E17" s="73" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="F17" s="73" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="G17" s="71" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="H17" s="70" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="I17" s="36" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="J17" s="9"/>
       <c r="K17" s="9" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="85.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="69"/>
       <c r="B18" s="69"/>
       <c r="C18" s="69" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="D18" s="69" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="E18" s="69" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="F18" s="69" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="G18" s="71" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="H18" s="70" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="I18" s="36" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="J18" s="9"/>
       <c r="K18" s="9" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="74.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4768,26 +4778,26 @@
         <v>43</v>
       </c>
       <c r="D19" s="69" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="E19" s="69" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="F19" s="69" t="s">
+        <v>415</v>
+      </c>
+      <c r="G19" s="71" t="s">
         <v>413</v>
       </c>
-      <c r="G19" s="71" t="s">
-        <v>411</v>
-      </c>
       <c r="H19" s="70" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="I19" s="36" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="J19" s="9"/>
       <c r="K19" s="9" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4797,22 +4807,22 @@
         <v>43</v>
       </c>
       <c r="D20" s="69" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="E20" s="69" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="F20" s="69" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="G20" s="71" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="H20" s="70" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="I20" s="72" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="J20" s="9"/>
       <c r="K20" s="9" t="s">

</xml_diff>

<commit_message>
Updated test data spreadsheet
</commit_message>
<xml_diff>
--- a/utils/testdata/DigitalSafariTESTDATA.xlsx
+++ b/utils/testdata/DigitalSafariTESTDATA.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="424">
   <si>
     <t xml:space="preserve">Information for Digital Safari web app</t>
   </si>
@@ -852,22 +852,25 @@
     <t xml:space="preserve">Crocodile Rock is an iconic Millport landmark. Although the rock itself has been in existence for millions of years it was only 106 years ago that its well-known face was painted on. The story goes that it was done by a local man with the name of Mr Brown, who was passing by after a lunchtime drink and saw the bare rock as a crocodile. He decided to return with a brush and paint and the well-loved crocodile came into existence! Crocodile rock can be located on the beach, opposite of the Dancing Midge Café.</t>
   </si>
   <si>
+    <t xml:space="preserve">https://commons.wikimedia.org/wiki/File:Crocodile_Rock,_Millport.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Draw your own crocodile masterpiece!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Largs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">55.7973317047214,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magnus the Viking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magnus is a steel statue located on the Largs seafront. He stands as a reminder that Largs was invaded by Vikings in the 1263 - it commemorates the Battle of Largs.</t>
+  </si>
+  <si>
     <t xml:space="preserve">In folder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Draw your own crocodile masterpiece!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Largs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">55.7973317047214,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Magnus the Viking</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Magnus is a steel statue located on the Largs seafront. He stands as a reminder that Largs was invaded by Vikings in the 1263 - it commemorates the Battle of Largs.</t>
   </si>
   <si>
     <t xml:space="preserve">Can you emulate his pose?</t>
@@ -2485,7 +2488,7 @@
   </sheetPr>
   <dimension ref="A3:J28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H11" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
@@ -3111,7 +3114,7 @@
   </sheetPr>
   <dimension ref="A3:K23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -3713,8 +3716,8 @@
   </sheetPr>
   <dimension ref="A3:K25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3837,11 +3840,11 @@
         <v>274</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="J6" s="9"/>
       <c r="K6" s="9" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="53.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3851,7 +3854,7 @@
         <v>42</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="E7" s="56" t="n">
         <v>55.6129152128045</v>
@@ -3860,17 +3863,17 @@
         <v>-4.48937852433251</v>
       </c>
       <c r="G7" s="18" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="H7" s="35" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="I7" s="57" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="J7" s="9"/>
       <c r="K7" s="9" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3880,26 +3883,26 @@
         <v>42</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="E8" s="56" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="F8" s="56" t="n">
         <v>-4.68434127824148</v>
       </c>
       <c r="G8" s="18" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="H8" s="35" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="J8" s="9"/>
       <c r="K8" s="9" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="43.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3909,26 +3912,26 @@
         <v>42</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="E9" s="56" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="F9" s="56" t="n">
         <v>-4.66607004947121</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="H9" s="35" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="I9" s="57" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="J9" s="9"/>
       <c r="K9" s="9" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="53.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3938,26 +3941,26 @@
         <v>42</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="E10" s="56" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="F10" s="56" t="n">
         <v>-4.84348802802478</v>
       </c>
       <c r="G10" s="18" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="H10" s="35" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="I10" s="57" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="J10" s="9"/>
       <c r="K10" s="9" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3967,26 +3970,26 @@
         <v>42</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="E11" s="56" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="F11" s="56" t="n">
         <v>-4.28600140104111</v>
       </c>
       <c r="G11" s="18" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="H11" s="35" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="J11" s="9"/>
       <c r="K11" s="9" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="43.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3996,22 +3999,22 @@
         <v>42</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="E12" s="56" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="F12" s="56" t="n">
         <v>-4.69848050344589</v>
       </c>
       <c r="G12" s="18" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="H12" s="35" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="I12" s="57" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="J12" s="9"/>
       <c r="K12" s="9" t="s">
@@ -4025,22 +4028,22 @@
         <v>42</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="E13" s="56" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="F13" s="56" t="n">
         <v>-4.74514981453443</v>
       </c>
       <c r="G13" s="18" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="H13" s="35" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="I13" s="57" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="J13" s="9"/>
       <c r="K13" s="9" t="s">
@@ -4054,22 +4057,22 @@
         <v>42</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="E14" s="56" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="F14" s="56" t="n">
         <v>-4.73272769919101</v>
       </c>
       <c r="G14" s="18" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="H14" s="35" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="J14" s="9"/>
       <c r="K14" s="9" t="s">
@@ -4083,26 +4086,26 @@
         <v>42</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="E15" s="56" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="F15" s="56" t="n">
         <v>-5.19201756110202</v>
       </c>
       <c r="G15" s="18" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="H15" s="35" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="I15" s="57" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="J15" s="9"/>
       <c r="K15" s="9" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="85.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4112,26 +4115,26 @@
         <v>42</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="E16" s="56" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="F16" s="56" t="n">
         <v>-4.45465267405307</v>
       </c>
       <c r="G16" s="18" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="H16" s="35" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="I16" s="57" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="J16" s="9"/>
       <c r="K16" s="9" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4141,26 +4144,26 @@
         <v>42</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="E17" s="56" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="F17" s="56" t="n">
         <v>-4.47766172987618</v>
       </c>
       <c r="G17" s="18" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="H17" s="35" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="I17" s="57" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="J17" s="9"/>
       <c r="K17" s="9" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4272,7 +4275,7 @@
     <mergeCell ref="A3:K3"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="I5" r:id="rId1" display="In folder"/>
+    <hyperlink ref="I5" r:id="rId1" display="https://commons.wikimedia.org/wiki/File:Crocodile_Rock,_Millport.jpg"/>
     <hyperlink ref="I7" r:id="rId2" display="In folder"/>
     <hyperlink ref="I9" r:id="rId3" display="In folder"/>
     <hyperlink ref="I10" r:id="rId4" display="In folder"/>
@@ -4356,7 +4359,7 @@
         <v>58</v>
       </c>
       <c r="I4" s="62" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="J4" s="63" t="s">
         <v>262</v>
@@ -4369,112 +4372,112 @@
       <c r="A5" s="65"/>
       <c r="B5" s="65"/>
       <c r="C5" s="65" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="D5" s="65" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="E5" s="65" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="F5" s="65" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="G5" s="66" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="H5" s="67" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="I5" s="68" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="J5" s="9"/>
       <c r="K5" s="9" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="53.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="69"/>
       <c r="B6" s="69"/>
       <c r="C6" s="69" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="D6" s="69" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="E6" s="69" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="F6" s="69" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="G6" s="69" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="H6" s="70" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="I6" s="36" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="J6" s="9"/>
       <c r="K6" s="9" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="64.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="69"/>
       <c r="B7" s="69"/>
       <c r="C7" s="69" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D7" s="69" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="E7" s="69" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="F7" s="69" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="G7" s="69" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="H7" s="70" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="I7" s="36" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="J7" s="9"/>
       <c r="K7" s="9" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="69"/>
       <c r="B8" s="69"/>
       <c r="C8" s="69" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="D8" s="69" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="E8" s="69" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="F8" s="69" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="G8" s="71" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="H8" s="70" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="I8" s="36" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="J8" s="9"/>
       <c r="K8" s="9" t="s">
@@ -4485,87 +4488,87 @@
       <c r="A9" s="69"/>
       <c r="B9" s="69"/>
       <c r="C9" s="69" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="D9" s="69" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="E9" s="69" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="F9" s="69" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="G9" s="71" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="H9" s="70" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="I9" s="36" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="J9" s="9"/>
       <c r="K9" s="9" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="85.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="69"/>
       <c r="B10" s="69"/>
       <c r="C10" s="69" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="D10" s="69" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="E10" s="69" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="F10" s="69" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="G10" s="71" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="H10" s="70" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="I10" s="36" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="J10" s="9"/>
       <c r="K10" s="9" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="53.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="69"/>
       <c r="B11" s="69"/>
       <c r="C11" s="69" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="D11" s="69" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="E11" s="69" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="F11" s="69" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="G11" s="71" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="H11" s="70" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="I11" s="72" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="J11" s="9"/>
       <c r="K11" s="9" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4575,51 +4578,51 @@
         <v>43</v>
       </c>
       <c r="D12" s="69" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="E12" s="69" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="F12" s="69" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="G12" s="71" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="H12" s="70" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="I12" s="36" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="J12" s="9"/>
       <c r="K12" s="9" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="85.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="69"/>
       <c r="B13" s="69"/>
       <c r="C13" s="69" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="D13" s="69" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="E13" s="69" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="F13" s="69" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="G13" s="71" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="H13" s="70" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="I13" s="36" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="J13" s="9"/>
       <c r="K13" s="9" t="s">
@@ -4633,142 +4636,142 @@
         <v>43</v>
       </c>
       <c r="D14" s="69" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="E14" s="69" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="F14" s="69" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="G14" s="71" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="H14" s="70" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="I14" s="36" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="J14" s="9"/>
       <c r="K14" s="9" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="64.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="69"/>
       <c r="B15" s="69"/>
       <c r="C15" s="69" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="D15" s="69" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="E15" s="69" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="F15" s="69" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="G15" s="71" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="H15" s="70" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="I15" s="36" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="J15" s="9"/>
       <c r="K15" s="9" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="69"/>
       <c r="B16" s="69"/>
       <c r="C16" s="69" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="D16" s="69" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="E16" s="69" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="F16" s="69" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="G16" s="71" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="H16" s="70" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="I16" s="36" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="J16" s="9"/>
       <c r="K16" s="9" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="69"/>
       <c r="B17" s="69"/>
       <c r="C17" s="69" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="D17" s="69" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="E17" s="73" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="F17" s="73" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="G17" s="71" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="H17" s="70" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="I17" s="36" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="J17" s="9"/>
       <c r="K17" s="9" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="85.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="69"/>
       <c r="B18" s="69"/>
       <c r="C18" s="69" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="D18" s="69" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="E18" s="69" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="F18" s="69" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="G18" s="71" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="H18" s="70" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="I18" s="36" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="J18" s="9"/>
       <c r="K18" s="9" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="74.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4778,26 +4781,26 @@
         <v>43</v>
       </c>
       <c r="D19" s="69" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="E19" s="69" t="s">
+        <v>415</v>
+      </c>
+      <c r="F19" s="69" t="s">
+        <v>416</v>
+      </c>
+      <c r="G19" s="71" t="s">
         <v>414</v>
       </c>
-      <c r="F19" s="69" t="s">
-        <v>415</v>
-      </c>
-      <c r="G19" s="71" t="s">
-        <v>413</v>
-      </c>
       <c r="H19" s="70" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="I19" s="36" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="J19" s="9"/>
       <c r="K19" s="9" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4807,22 +4810,22 @@
         <v>43</v>
       </c>
       <c r="D20" s="69" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="E20" s="69" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="F20" s="69" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="G20" s="71" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="H20" s="70" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="I20" s="72" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="J20" s="9"/>
       <c r="K20" s="9" t="s">

</xml_diff>